<commit_message>
implemented update and tested it
</commit_message>
<xml_diff>
--- a/test_data/middleware_test_results.xlsx
+++ b/test_data/middleware_test_results.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgedinicola/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgedinicola/Desktop/TDRB-Middleware-Extension/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F1D7B9-974A-424D-8599-1650F2F6AF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C100363-D962-5145-A6F9-8A7742FF5C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="4700" windowWidth="28040" windowHeight="17440" xr2:uid="{BD2E64C6-9971-2049-987A-C9A8CB2241EA}"/>
+    <workbookView xWindow="20340" yWindow="4980" windowWidth="28040" windowHeight="17440" xr2:uid="{BD2E64C6-9971-2049-987A-C9A8CB2241EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>NEW</t>
   </si>
@@ -59,6 +59,123 @@
   </si>
   <si>
     <t>In Seconds</t>
+  </si>
+  <si>
+    <t>real 2m1.124s</t>
+  </si>
+  <si>
+    <t>real 2m0.683s</t>
+  </si>
+  <si>
+    <t>real 2m0.779s</t>
+  </si>
+  <si>
+    <t>real 2m0.407s</t>
+  </si>
+  <si>
+    <t>real 2m0.431s</t>
+  </si>
+  <si>
+    <t>real 2m0.687s</t>
+  </si>
+  <si>
+    <t>real 2m0.277s</t>
+  </si>
+  <si>
+    <t>real 2m0.855s</t>
+  </si>
+  <si>
+    <t>real 2m0.280s</t>
+  </si>
+  <si>
+    <t>real 2m0.454s</t>
+  </si>
+  <si>
+    <t>real 2m0.345s</t>
+  </si>
+  <si>
+    <t>real 2m0.364s</t>
+  </si>
+  <si>
+    <t>real 2m0.626s</t>
+  </si>
+  <si>
+    <t>real 2m0.694s</t>
+  </si>
+  <si>
+    <t>real 2m2.223s</t>
+  </si>
+  <si>
+    <t>real 2m2.071s</t>
+  </si>
+  <si>
+    <t>real 2m1.023s</t>
+  </si>
+  <si>
+    <t>real 2m0.333s</t>
+  </si>
+  <si>
+    <t>real 2m0.290s</t>
+  </si>
+  <si>
+    <t>real 2m0.306s</t>
+  </si>
+  <si>
+    <t>real 2m0.546s</t>
+  </si>
+  <si>
+    <t>real 2m1.087s</t>
+  </si>
+  <si>
+    <t>real 2m0.222s</t>
+  </si>
+  <si>
+    <t>real 2m0.220s</t>
+  </si>
+  <si>
+    <t>real 2m0.170s</t>
+  </si>
+  <si>
+    <t>real 2m0.764s</t>
+  </si>
+  <si>
+    <t>real 2m0.744s</t>
+  </si>
+  <si>
+    <t>real 2m0.382s</t>
+  </si>
+  <si>
+    <t>real 2m1.110s</t>
+  </si>
+  <si>
+    <t>real 2m0.406s</t>
+  </si>
+  <si>
+    <t>real 2m0.360s</t>
+  </si>
+  <si>
+    <t>real 2m0.657s</t>
+  </si>
+  <si>
+    <t>real 2m0.976s</t>
+  </si>
+  <si>
+    <t>real 2m1.219s</t>
+  </si>
+  <si>
+    <t>real 2m2.711s</t>
+  </si>
+  <si>
+    <t>real 2m1.193s</t>
+  </si>
+  <si>
+    <t>real 2m1.993s</t>
+  </si>
+  <si>
+    <t>real 2m1.306s</t>
+  </si>
+  <si>
+    <t>real 2m2.135s</t>
   </si>
 </sst>
 </file>
@@ -66,7 +183,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -135,12 +252,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -457,20 +574,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AC3783-C63C-AE47-8CCA-EA7F35C5FC8A}">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -507,7 +624,7 @@
       <c r="L4" s="10"/>
       <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="6">
         <v>3.1709999999999998</v>
       </c>
@@ -517,6 +634,9 @@
       <c r="D5" s="7">
         <v>9.74</v>
       </c>
+      <c r="E5" s="6">
+        <v>6.41</v>
+      </c>
       <c r="G5">
         <v>117.509</v>
       </c>
@@ -526,9 +646,26 @@
       <c r="I5">
         <v>123.31</v>
       </c>
+      <c r="J5">
+        <v>121.124</v>
+      </c>
       <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5" t="str">
+        <f>RIGHT(L5,6)</f>
+        <v>1.124s</v>
+      </c>
+      <c r="P5" t="str">
+        <f>LEFT(O5,5)</f>
+        <v>1.124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B6" s="6">
         <v>3.153</v>
       </c>
@@ -538,6 +675,9 @@
       <c r="D6" s="7">
         <v>9.7539999999999996</v>
       </c>
+      <c r="E6" s="6">
+        <v>6.391</v>
+      </c>
       <c r="G6">
         <v>117.544</v>
       </c>
@@ -547,9 +687,26 @@
       <c r="I6">
         <v>122.05200000000001</v>
       </c>
+      <c r="J6">
+        <v>120.68300000000001</v>
+      </c>
       <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" ref="O6:O44" si="0">RIGHT(L6,6)</f>
+        <v>0.683s</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" ref="P6:P44" si="1">LEFT(O6,5)</f>
+        <v>0.683</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7" s="6">
         <v>3.145</v>
       </c>
@@ -559,6 +716,9 @@
       <c r="D7" s="7">
         <v>9.7110000000000003</v>
       </c>
+      <c r="E7" s="6">
+        <v>6.407</v>
+      </c>
       <c r="G7">
         <v>117.739</v>
       </c>
@@ -568,9 +728,26 @@
       <c r="I7">
         <v>120.964</v>
       </c>
+      <c r="J7">
+        <v>120.779</v>
+      </c>
       <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="0"/>
+        <v>0.779s</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="1"/>
+        <v>0.779</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B8" s="6">
         <v>3.1640000000000001</v>
       </c>
@@ -580,6 +757,9 @@
       <c r="D8" s="7">
         <v>9.6809999999999992</v>
       </c>
+      <c r="E8" s="6">
+        <v>6.4160000000000004</v>
+      </c>
       <c r="G8">
         <v>117.53999999999999</v>
       </c>
@@ -589,9 +769,26 @@
       <c r="I8">
         <v>69.956999999999994</v>
       </c>
+      <c r="J8">
+        <v>120.407</v>
+      </c>
       <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="0"/>
+        <v>0.407s</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="1"/>
+        <v>0.407</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9" s="6">
         <v>3.1579999999999999</v>
       </c>
@@ -601,6 +798,9 @@
       <c r="D9" s="7">
         <v>9.7149999999999999</v>
       </c>
+      <c r="E9" s="6">
+        <v>6.4240000000000004</v>
+      </c>
       <c r="G9">
         <v>117.70699999999999</v>
       </c>
@@ -610,9 +810,26 @@
       <c r="I9">
         <v>68.622</v>
       </c>
+      <c r="J9">
+        <v>120.431</v>
+      </c>
       <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="0"/>
+        <v>0.431s</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="1"/>
+        <v>0.431</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10" s="6">
         <v>3.1469999999999998</v>
       </c>
@@ -622,6 +839,9 @@
       <c r="D10" s="7">
         <v>9.6760000000000002</v>
       </c>
+      <c r="E10" s="6">
+        <v>6.4420000000000002</v>
+      </c>
       <c r="G10">
         <v>117.65</v>
       </c>
@@ -631,9 +851,26 @@
       <c r="I10">
         <v>67.537999999999997</v>
       </c>
+      <c r="J10">
+        <v>120.687</v>
+      </c>
       <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="0"/>
+        <v>0.687s</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="1"/>
+        <v>0.687</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="6">
         <v>3.161</v>
       </c>
@@ -643,6 +880,9 @@
       <c r="D11" s="7">
         <v>9.702</v>
       </c>
+      <c r="E11" s="6">
+        <v>6.4450000000000003</v>
+      </c>
       <c r="G11">
         <v>117.59899999999999</v>
       </c>
@@ -652,9 +892,26 @@
       <c r="I11">
         <v>66.358999999999995</v>
       </c>
+      <c r="J11">
+        <v>120.277</v>
+      </c>
       <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="0"/>
+        <v>0.277s</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="1"/>
+        <v>0.277</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="6">
         <v>3.1659999999999999</v>
       </c>
@@ -664,6 +921,9 @@
       <c r="D12" s="7">
         <v>9.68</v>
       </c>
+      <c r="E12" s="6">
+        <v>6.4160000000000004</v>
+      </c>
       <c r="G12">
         <v>117.682</v>
       </c>
@@ -673,9 +933,26 @@
       <c r="I12">
         <v>65.144999999999996</v>
       </c>
+      <c r="J12">
+        <v>120.855</v>
+      </c>
       <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12">
+        <v>2</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="0"/>
+        <v>0.855s</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="1"/>
+        <v>0.855</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="6">
         <v>3.1949999999999998</v>
       </c>
@@ -685,6 +962,9 @@
       <c r="D13" s="7">
         <v>9.6750000000000007</v>
       </c>
+      <c r="E13" s="6">
+        <v>6.4279999999999999</v>
+      </c>
       <c r="G13">
         <v>117.815</v>
       </c>
@@ -694,9 +974,26 @@
       <c r="I13">
         <v>64.224999999999994</v>
       </c>
+      <c r="J13">
+        <v>120.28</v>
+      </c>
       <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="0"/>
+        <v>0.280s</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="1"/>
+        <v>0.280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="6">
         <v>3.242</v>
       </c>
@@ -706,6 +1003,9 @@
       <c r="D14" s="7">
         <v>9.73</v>
       </c>
+      <c r="E14" s="6">
+        <v>6.4020000000000001</v>
+      </c>
       <c r="G14">
         <v>117.53999999999999</v>
       </c>
@@ -715,9 +1015,26 @@
       <c r="I14">
         <v>62.991</v>
       </c>
+      <c r="J14">
+        <v>120.45399999999999</v>
+      </c>
       <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L14" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="0"/>
+        <v>0.454s</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="1"/>
+        <v>0.454</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="6">
         <v>3.1709999999999998</v>
       </c>
@@ -727,6 +1044,9 @@
       <c r="D15" s="7">
         <v>9.7100000000000009</v>
       </c>
+      <c r="E15" s="6">
+        <v>6.4009999999999998</v>
+      </c>
       <c r="G15">
         <v>117.51599999999999</v>
       </c>
@@ -736,9 +1056,26 @@
       <c r="I15">
         <v>61.79</v>
       </c>
+      <c r="J15">
+        <v>120.345</v>
+      </c>
       <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="0"/>
+        <v>0.345s</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="1"/>
+        <v>0.345</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" s="6">
         <v>3.1859999999999999</v>
       </c>
@@ -748,6 +1085,9 @@
       <c r="D16" s="7">
         <v>9.6950000000000003</v>
       </c>
+      <c r="E16" s="6">
+        <v>6.4059999999999997</v>
+      </c>
       <c r="G16">
         <v>117.471</v>
       </c>
@@ -757,9 +1097,26 @@
       <c r="I16">
         <v>60.631</v>
       </c>
+      <c r="J16">
+        <v>120.364</v>
+      </c>
       <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L16" t="s">
+        <v>19</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="0"/>
+        <v>0.364s</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="1"/>
+        <v>0.364</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17" s="6">
         <v>3.1440000000000001</v>
       </c>
@@ -769,6 +1126,9 @@
       <c r="D17" s="7">
         <v>9.7089999999999996</v>
       </c>
+      <c r="E17" s="6">
+        <v>6.4059999999999997</v>
+      </c>
       <c r="G17">
         <v>117.52799999999999</v>
       </c>
@@ -778,9 +1138,26 @@
       <c r="I17">
         <v>69.539000000000001</v>
       </c>
+      <c r="J17">
+        <v>120.626</v>
+      </c>
       <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="0"/>
+        <v>0.626s</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" si="1"/>
+        <v>0.626</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B18" s="6">
         <v>3.1789999999999998</v>
       </c>
@@ -790,6 +1167,9 @@
       <c r="D18" s="7">
         <v>9.6649999999999991</v>
       </c>
+      <c r="E18" s="6">
+        <v>6.43</v>
+      </c>
       <c r="G18">
         <v>117.64400000000001</v>
       </c>
@@ -799,9 +1179,26 @@
       <c r="I18">
         <v>68.462000000000003</v>
       </c>
+      <c r="J18">
+        <v>120.694</v>
+      </c>
       <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L18" t="s">
+        <v>21</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="0"/>
+        <v>0.694s</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="1"/>
+        <v>0.694</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B19" s="6">
         <v>3.14</v>
       </c>
@@ -811,6 +1208,9 @@
       <c r="D19" s="7">
         <v>9.6660000000000004</v>
       </c>
+      <c r="E19" s="6">
+        <v>6.4</v>
+      </c>
       <c r="G19">
         <v>117.73599999999999</v>
       </c>
@@ -820,9 +1220,26 @@
       <c r="I19">
         <v>67.135999999999996</v>
       </c>
+      <c r="J19">
+        <v>122.223</v>
+      </c>
       <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L19" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="0"/>
+        <v>2.223s</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="1"/>
+        <v>2.223</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B20" s="6">
         <v>3.1680000000000001</v>
       </c>
@@ -832,6 +1249,9 @@
       <c r="D20" s="7">
         <v>9.6989999999999998</v>
       </c>
+      <c r="E20" s="6">
+        <v>6.41</v>
+      </c>
       <c r="G20">
         <v>117.93299999999999</v>
       </c>
@@ -841,9 +1261,26 @@
       <c r="I20">
         <v>66.221999999999994</v>
       </c>
+      <c r="J20">
+        <v>122.071</v>
+      </c>
       <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>23</v>
+      </c>
+      <c r="N20">
+        <v>2</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="0"/>
+        <v>2.071s</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="1"/>
+        <v>2.071</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B21" s="6">
         <v>3.1739999999999999</v>
       </c>
@@ -853,6 +1290,9 @@
       <c r="D21" s="7">
         <v>9.7089999999999996</v>
       </c>
+      <c r="E21" s="6">
+        <v>6.3760000000000003</v>
+      </c>
       <c r="G21">
         <v>117.63499999999999</v>
       </c>
@@ -862,9 +1302,26 @@
       <c r="I21">
         <v>65.100999999999999</v>
       </c>
+      <c r="J21">
+        <v>121.023</v>
+      </c>
       <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L21" t="s">
+        <v>24</v>
+      </c>
+      <c r="N21">
+        <v>2</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="0"/>
+        <v>1.023s</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="1"/>
+        <v>1.023</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B22" s="6">
         <v>3.1429999999999998</v>
       </c>
@@ -874,6 +1331,9 @@
       <c r="D22" s="7">
         <v>9.7379999999999995</v>
       </c>
+      <c r="E22" s="6">
+        <v>6.4269999999999996</v>
+      </c>
       <c r="G22">
         <v>117.613</v>
       </c>
@@ -883,9 +1343,26 @@
       <c r="I22">
         <v>63.841000000000001</v>
       </c>
+      <c r="J22">
+        <v>120.333</v>
+      </c>
       <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L22" t="s">
+        <v>25</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="0"/>
+        <v>0.333s</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" si="1"/>
+        <v>0.333</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B23" s="6">
         <v>3.17</v>
       </c>
@@ -895,6 +1372,9 @@
       <c r="D23" s="7">
         <v>9.7880000000000003</v>
       </c>
+      <c r="E23" s="6">
+        <v>6.42</v>
+      </c>
       <c r="G23">
         <v>117.49199999999999</v>
       </c>
@@ -904,9 +1384,26 @@
       <c r="I23">
         <v>62.548999999999999</v>
       </c>
+      <c r="J23">
+        <v>120.29</v>
+      </c>
       <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L23" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23">
+        <v>2</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="0"/>
+        <v>0.290s</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="1"/>
+        <v>0.290</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B24" s="6">
         <v>3.157</v>
       </c>
@@ -916,6 +1413,9 @@
       <c r="D24" s="7">
         <v>9.8019999999999996</v>
       </c>
+      <c r="E24" s="6">
+        <v>6.407</v>
+      </c>
       <c r="G24">
         <v>117.61099999999999</v>
       </c>
@@ -925,9 +1425,26 @@
       <c r="I24">
         <v>61.415999999999997</v>
       </c>
+      <c r="J24">
+        <v>120.306</v>
+      </c>
       <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L24" t="s">
+        <v>27</v>
+      </c>
+      <c r="N24">
+        <v>2</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="0"/>
+        <v>0.306s</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="1"/>
+        <v>0.306</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="6">
         <v>3.1509999999999998</v>
       </c>
@@ -937,6 +1454,9 @@
       <c r="D25" s="7">
         <v>9.74</v>
       </c>
+      <c r="E25" s="6">
+        <v>6.4269999999999996</v>
+      </c>
       <c r="G25">
         <v>117.85900000000001</v>
       </c>
@@ -946,9 +1466,26 @@
       <c r="I25">
         <v>60.472000000000001</v>
       </c>
+      <c r="J25">
+        <v>120.54600000000001</v>
+      </c>
       <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L25" t="s">
+        <v>28</v>
+      </c>
+      <c r="N25">
+        <v>2</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="0"/>
+        <v>0.546s</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" si="1"/>
+        <v>0.546</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B26" s="6">
         <v>3.1589999999999998</v>
       </c>
@@ -958,6 +1495,9 @@
       <c r="D26" s="7">
         <v>9.6880000000000006</v>
       </c>
+      <c r="E26" s="6">
+        <v>6.4020000000000001</v>
+      </c>
       <c r="G26">
         <v>117.988</v>
       </c>
@@ -967,9 +1507,26 @@
       <c r="I26">
         <v>69.206999999999994</v>
       </c>
+      <c r="J26">
+        <v>121.087</v>
+      </c>
       <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L26" t="s">
+        <v>29</v>
+      </c>
+      <c r="N26">
+        <v>2</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="0"/>
+        <v>1.087s</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="1"/>
+        <v>1.087</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B27" s="6">
         <v>3.1360000000000001</v>
       </c>
@@ -979,6 +1536,9 @@
       <c r="D27" s="7">
         <v>9.7620000000000005</v>
       </c>
+      <c r="E27" s="6">
+        <v>6.399</v>
+      </c>
       <c r="G27">
         <v>117.73599999999999</v>
       </c>
@@ -988,9 +1548,26 @@
       <c r="I27">
         <v>68.188999999999993</v>
       </c>
+      <c r="J27">
+        <v>120.22199999999999</v>
+      </c>
       <c r="K27" s="6"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L27" t="s">
+        <v>30</v>
+      </c>
+      <c r="N27">
+        <v>2</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="0"/>
+        <v>0.222s</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" si="1"/>
+        <v>0.222</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B28" s="6">
         <v>3.1589999999999998</v>
       </c>
@@ -1000,6 +1577,9 @@
       <c r="D28" s="7">
         <v>9.6980000000000004</v>
       </c>
+      <c r="E28" s="6">
+        <v>6.3550000000000004</v>
+      </c>
       <c r="G28">
         <v>117.753</v>
       </c>
@@ -1009,9 +1589,26 @@
       <c r="I28">
         <v>63.829000000000001</v>
       </c>
+      <c r="J28">
+        <v>120.22</v>
+      </c>
       <c r="K28" s="6"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L28" t="s">
+        <v>31</v>
+      </c>
+      <c r="N28">
+        <v>2</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="0"/>
+        <v>0.220s</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" si="1"/>
+        <v>0.220</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29" s="6">
         <v>3.1640000000000001</v>
       </c>
@@ -1021,6 +1618,9 @@
       <c r="D29" s="7">
         <v>9.718</v>
       </c>
+      <c r="E29" s="6">
+        <v>6.5140000000000002</v>
+      </c>
       <c r="G29">
         <v>117.60300000000001</v>
       </c>
@@ -1030,9 +1630,26 @@
       <c r="I29">
         <v>69.88</v>
       </c>
+      <c r="J29">
+        <v>120.17</v>
+      </c>
       <c r="K29" s="6"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L29" t="s">
+        <v>32</v>
+      </c>
+      <c r="N29">
+        <v>2</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="0"/>
+        <v>0.170s</v>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" si="1"/>
+        <v>0.170</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="6">
         <v>3.26</v>
       </c>
@@ -1042,6 +1659,9 @@
       <c r="D30" s="7">
         <v>9.6829999999999998</v>
       </c>
+      <c r="E30" s="6">
+        <v>6.4809999999999999</v>
+      </c>
       <c r="G30">
         <v>117.837</v>
       </c>
@@ -1051,9 +1671,26 @@
       <c r="I30">
         <v>122.81100000000001</v>
       </c>
+      <c r="J30">
+        <v>120.764</v>
+      </c>
       <c r="K30" s="6"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L30" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30">
+        <v>2</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="0"/>
+        <v>0.764s</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" si="1"/>
+        <v>0.764</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B31" s="6">
         <v>3.286</v>
       </c>
@@ -1063,6 +1700,9 @@
       <c r="D31" s="7">
         <v>9.6509999999999998</v>
       </c>
+      <c r="E31" s="6">
+        <v>6.4059999999999997</v>
+      </c>
       <c r="G31">
         <v>117.637</v>
       </c>
@@ -1072,9 +1712,26 @@
       <c r="I31">
         <v>128.69900000000001</v>
       </c>
+      <c r="J31">
+        <v>120.744</v>
+      </c>
       <c r="K31" s="6"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L31" t="s">
+        <v>34</v>
+      </c>
+      <c r="N31">
+        <v>2</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="0"/>
+        <v>0.744s</v>
+      </c>
+      <c r="P31" t="str">
+        <f t="shared" si="1"/>
+        <v>0.744</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B32" s="6">
         <v>3.2789999999999999</v>
       </c>
@@ -1084,6 +1741,9 @@
       <c r="D32" s="7">
         <v>9.6969999999999992</v>
       </c>
+      <c r="E32" s="6">
+        <v>6.4160000000000004</v>
+      </c>
       <c r="G32">
         <v>117.556</v>
       </c>
@@ -1093,9 +1753,26 @@
       <c r="I32">
         <v>122.48</v>
       </c>
+      <c r="J32">
+        <v>120.38200000000001</v>
+      </c>
       <c r="K32" s="6"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L32" t="s">
+        <v>35</v>
+      </c>
+      <c r="N32">
+        <v>2</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="0"/>
+        <v>0.382s</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="1"/>
+        <v>0.382</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B33" s="6">
         <v>3.28</v>
       </c>
@@ -1105,6 +1782,9 @@
       <c r="D33" s="7">
         <v>9.6820000000000004</v>
       </c>
+      <c r="E33" s="6">
+        <v>6.3929999999999998</v>
+      </c>
       <c r="G33">
         <v>117.58799999999999</v>
       </c>
@@ -1114,9 +1794,26 @@
       <c r="I33">
         <v>121.40300000000001</v>
       </c>
+      <c r="J33">
+        <v>121.11</v>
+      </c>
       <c r="K33" s="6"/>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>36</v>
+      </c>
+      <c r="N33">
+        <v>2</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="0"/>
+        <v>1.110s</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" si="1"/>
+        <v>1.110</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B34" s="6">
         <v>3.2909999999999999</v>
       </c>
@@ -1126,6 +1823,9 @@
       <c r="D34" s="7">
         <v>9.6679999999999993</v>
       </c>
+      <c r="E34" s="6">
+        <v>6.4509999999999996</v>
+      </c>
       <c r="G34">
         <v>117.71899999999999</v>
       </c>
@@ -1135,9 +1835,26 @@
       <c r="I34">
         <v>129.81</v>
       </c>
+      <c r="J34">
+        <v>120.40600000000001</v>
+      </c>
       <c r="K34" s="6"/>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L34" t="s">
+        <v>37</v>
+      </c>
+      <c r="N34">
+        <v>2</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="0"/>
+        <v>0.406s</v>
+      </c>
+      <c r="P34" t="str">
+        <f t="shared" si="1"/>
+        <v>0.406</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B35" s="6">
         <v>3.226</v>
       </c>
@@ -1147,6 +1864,9 @@
       <c r="D35" s="7">
         <v>9.6489999999999991</v>
       </c>
+      <c r="E35" s="6">
+        <v>6.4640000000000004</v>
+      </c>
       <c r="G35">
         <v>117.675</v>
       </c>
@@ -1156,9 +1876,26 @@
       <c r="I35">
         <v>128.69200000000001</v>
       </c>
+      <c r="J35">
+        <v>120.333</v>
+      </c>
       <c r="K35" s="6"/>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L35" t="s">
+        <v>25</v>
+      </c>
+      <c r="N35">
+        <v>2</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="0"/>
+        <v>0.333s</v>
+      </c>
+      <c r="P35" t="str">
+        <f t="shared" si="1"/>
+        <v>0.333</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B36" s="6">
         <v>3.202</v>
       </c>
@@ -1168,6 +1905,9 @@
       <c r="D36" s="7">
         <v>9.6890000000000001</v>
       </c>
+      <c r="E36" s="6">
+        <v>6.4279999999999999</v>
+      </c>
       <c r="G36">
         <v>117.547</v>
       </c>
@@ -1177,9 +1917,26 @@
       <c r="I36">
         <v>67.721000000000004</v>
       </c>
+      <c r="J36">
+        <v>120.36</v>
+      </c>
       <c r="K36" s="6"/>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L36" t="s">
+        <v>38</v>
+      </c>
+      <c r="N36">
+        <v>2</v>
+      </c>
+      <c r="O36" t="str">
+        <f t="shared" si="0"/>
+        <v>0.360s</v>
+      </c>
+      <c r="P36" t="str">
+        <f t="shared" si="1"/>
+        <v>0.360</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B37" s="6">
         <v>3.1549999999999998</v>
       </c>
@@ -1189,6 +1946,9 @@
       <c r="D37" s="7">
         <v>9.6739999999999995</v>
       </c>
+      <c r="E37" s="6">
+        <v>6.4630000000000001</v>
+      </c>
       <c r="G37">
         <v>117.60499999999999</v>
       </c>
@@ -1198,9 +1958,26 @@
       <c r="I37">
         <v>126.672</v>
       </c>
+      <c r="J37">
+        <v>120.657</v>
+      </c>
       <c r="K37" s="6"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L37" t="s">
+        <v>39</v>
+      </c>
+      <c r="N37">
+        <v>2</v>
+      </c>
+      <c r="O37" t="str">
+        <f t="shared" si="0"/>
+        <v>0.657s</v>
+      </c>
+      <c r="P37" t="str">
+        <f t="shared" si="1"/>
+        <v>0.657</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B38" s="6">
         <v>3.15</v>
       </c>
@@ -1210,6 +1987,9 @@
       <c r="D38" s="7">
         <v>9.6379999999999999</v>
       </c>
+      <c r="E38" s="6">
+        <v>6.4409999999999998</v>
+      </c>
       <c r="G38">
         <v>117.907</v>
       </c>
@@ -1219,9 +1999,26 @@
       <c r="I38">
         <v>65.847999999999999</v>
       </c>
+      <c r="J38">
+        <v>120.976</v>
+      </c>
       <c r="K38" s="6"/>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L38" t="s">
+        <v>40</v>
+      </c>
+      <c r="N38">
+        <v>2</v>
+      </c>
+      <c r="O38" t="str">
+        <f t="shared" si="0"/>
+        <v>0.976s</v>
+      </c>
+      <c r="P38" t="str">
+        <f t="shared" si="1"/>
+        <v>0.976</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B39" s="6">
         <v>3.17</v>
       </c>
@@ -1231,6 +2028,9 @@
       <c r="D39" s="7">
         <v>9.7460000000000004</v>
       </c>
+      <c r="E39" s="6">
+        <v>6.4130000000000003</v>
+      </c>
       <c r="G39">
         <v>117.753</v>
       </c>
@@ -1240,9 +2040,26 @@
       <c r="I39">
         <v>184.98099999999999</v>
       </c>
+      <c r="J39">
+        <v>121.21899999999999</v>
+      </c>
       <c r="K39" s="6"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L39" t="s">
+        <v>41</v>
+      </c>
+      <c r="N39">
+        <v>2</v>
+      </c>
+      <c r="O39" t="str">
+        <f t="shared" si="0"/>
+        <v>1.219s</v>
+      </c>
+      <c r="P39" t="str">
+        <f t="shared" si="1"/>
+        <v>1.219</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B40" s="6">
         <v>3.1859999999999999</v>
       </c>
@@ -1252,6 +2069,9 @@
       <c r="D40" s="7">
         <v>9.6639999999999997</v>
       </c>
+      <c r="E40" s="6">
+        <v>6.38</v>
+      </c>
       <c r="G40">
         <v>117.71299999999999</v>
       </c>
@@ -1261,9 +2081,26 @@
       <c r="I40">
         <v>63.198</v>
       </c>
+      <c r="J40">
+        <v>122.711</v>
+      </c>
       <c r="K40" s="6"/>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L40" t="s">
+        <v>42</v>
+      </c>
+      <c r="N40">
+        <v>2</v>
+      </c>
+      <c r="O40" t="str">
+        <f t="shared" si="0"/>
+        <v>2.711s</v>
+      </c>
+      <c r="P40" t="str">
+        <f t="shared" si="1"/>
+        <v>2.711</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B41" s="6">
         <v>3.19</v>
       </c>
@@ -1273,6 +2110,9 @@
       <c r="D41" s="7">
         <v>9.6259999999999994</v>
       </c>
+      <c r="E41" s="6">
+        <v>6.3860000000000001</v>
+      </c>
       <c r="G41">
         <v>117.6</v>
       </c>
@@ -1282,9 +2122,26 @@
       <c r="I41">
         <v>121.086</v>
       </c>
+      <c r="J41">
+        <v>121.193</v>
+      </c>
       <c r="K41" s="6"/>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L41" t="s">
+        <v>43</v>
+      </c>
+      <c r="N41">
+        <v>2</v>
+      </c>
+      <c r="O41" t="str">
+        <f t="shared" si="0"/>
+        <v>1.193s</v>
+      </c>
+      <c r="P41" t="str">
+        <f t="shared" si="1"/>
+        <v>1.193</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B42" s="6">
         <v>3.1819999999999999</v>
       </c>
@@ -1294,15 +2151,35 @@
       <c r="D42" s="7">
         <v>9.7230000000000008</v>
       </c>
+      <c r="E42" s="6">
+        <v>6.4089999999999998</v>
+      </c>
       <c r="G42">
         <v>117.71299999999999</v>
       </c>
       <c r="I42">
         <v>65.792000000000002</v>
       </c>
+      <c r="J42">
+        <v>121.99299999999999</v>
+      </c>
       <c r="K42" s="6"/>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L42" t="s">
+        <v>44</v>
+      </c>
+      <c r="N42">
+        <v>2</v>
+      </c>
+      <c r="O42" t="str">
+        <f t="shared" si="0"/>
+        <v>1.993s</v>
+      </c>
+      <c r="P42" t="str">
+        <f t="shared" si="1"/>
+        <v>1.993</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B43" s="6">
         <v>3.1840000000000002</v>
       </c>
@@ -1312,15 +2189,35 @@
       <c r="D43" s="7">
         <v>9.8040000000000003</v>
       </c>
+      <c r="E43" s="6">
+        <v>6.3949999999999996</v>
+      </c>
       <c r="G43">
         <v>117.675</v>
       </c>
       <c r="I43">
         <v>66.787000000000006</v>
       </c>
+      <c r="J43">
+        <v>121.306</v>
+      </c>
       <c r="K43" s="6"/>
-    </row>
-    <row r="44" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L43" t="s">
+        <v>45</v>
+      </c>
+      <c r="N43">
+        <v>2</v>
+      </c>
+      <c r="O43" t="str">
+        <f t="shared" si="0"/>
+        <v>1.306s</v>
+      </c>
+      <c r="P43" t="str">
+        <f t="shared" si="1"/>
+        <v>1.306</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5">
         <v>3.1539999999999999</v>
       </c>
@@ -1329,6 +2226,9 @@
       </c>
       <c r="D44" s="8">
         <v>9.8320000000000007</v>
+      </c>
+      <c r="E44" s="5">
+        <v>6.4130000000000003</v>
       </c>
       <c r="G44" s="3">
         <v>117.30199999999999</v>
@@ -1337,9 +2237,26 @@
       <c r="I44" s="3">
         <v>121.95699999999999</v>
       </c>
+      <c r="J44" s="3">
+        <v>122.13500000000001</v>
+      </c>
       <c r="K44" s="6"/>
-    </row>
-    <row r="45" spans="2:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="L44" t="s">
+        <v>46</v>
+      </c>
+      <c r="N44">
+        <v>2</v>
+      </c>
+      <c r="O44" t="str">
+        <f t="shared" si="0"/>
+        <v>2.135s</v>
+      </c>
+      <c r="P44" t="str">
+        <f t="shared" si="1"/>
+        <v>2.135</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B45" s="9">
         <f>AVERAGE(B5:B44)</f>
         <v>3.1824500000000002</v>
@@ -1352,6 +2269,10 @@
         <f>AVERAGE(D5:D44)</f>
         <v>9.7069249999999982</v>
       </c>
+      <c r="E45" s="9">
+        <f>AVERAGE(E5:E44)</f>
+        <v>6.4174999999999995</v>
+      </c>
       <c r="G45" s="1">
         <f>AVERAGE(G5:G44)</f>
         <v>117.65675000000002</v>
@@ -1364,8 +2285,12 @@
         <f>AVERAGE(I5:I44)</f>
         <v>86.184099999999958</v>
       </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="J45" s="1">
+        <f>AVERAGE(J5:J44)</f>
+        <v>120.81965000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>

</xml_diff>